<commit_message>
finished implementation of conditional formatting
finished implementation of conditional formatting
</commit_message>
<xml_diff>
--- a/modified_output.xlsx
+++ b/modified_output.xlsx
@@ -64,6 +64,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00ffff00"/>
+          <bgColor rgb="00ffff00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -739,7 +749,42 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="7">
+  <conditionalFormatting sqref="A2:A1000">
+    <cfRule type="expression" priority="1" dxfId="0" stopIfTrue="1">
+      <formula>=AND(ISBLANK(A2),OR(NOT(ISBLANK(B2)),NOT(ISBLANK(C2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F1000">
+    <cfRule type="expression" priority="2" dxfId="0" stopIfTrue="1">
+      <formula>=AND(NOT(AND(LEN(F2)=12,ISNUMBER(VALUE(LEFT(F2,2))),MID(F2,3,1)="-",ISNUMBER(VALUE(MID(F2,4,6))),MID(F2,10,1)="-",ISNUMBER(VALUE(RIGHT(F2,2))))),NOT(AND(LEN(F2)=10,ISNUMBER(VALUE(F2)))),AND(ISBLANK(F2),NOT(ISBLANK(G2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J1000">
+    <cfRule type="expression" priority="3" dxfId="0" stopIfTrue="1">
+      <formula>=AND(NOT(LEN(J2)=2),NOT(ISBLANK(J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M1000">
+    <cfRule type="expression" priority="4" dxfId="0" stopIfTrue="1">
+      <formula>=OR(NOT(AND(IFERROR(M2&lt;=$K2,FALSE),IFERROR($M2+$P2+$Q2+$S2&lt;=$K2,FALSE))),AND(NOT(ISBLANK(M2)),NOT(ISNUMBER(M2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:S1000">
+    <cfRule type="expression" priority="5" dxfId="0" stopIfTrue="1">
+      <formula>=OR(NOT(AND(IFERROR(M2&lt;=$K2,FALSE),IFERROR($M2+$P2+$Q2+$S2&lt;=$K2,FALSE))),AND(NOT(ISBLANK(M2)),NOT(ISNUMBER(M2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P1000">
+    <cfRule type="expression" priority="6" dxfId="0" stopIfTrue="1">
+      <formula>=OR(NOT(AND(IFERROR(M2&lt;=$K2,FALSE),IFERROR($M2+$P2+$Q2+$S2&lt;=$K2,FALSE))),AND(NOT(ISBLANK(M2)),NOT(ISNUMBER(M2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q1000">
+    <cfRule type="expression" priority="7" dxfId="0" stopIfTrue="1">
+      <formula>=OR(AND(NOT(ISBLANK(Q2)),NOT(ISNUMBER(Q2))),AND(ISBLANK(Q2),NOT(ISBLANK(R2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="9">
     <dataValidation sqref="F2:F1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" error="Input must be in valid medicaid id format (**-******-**)" type="custom">
       <formula1>=OR(AND(LEN(F1)=12,ISNUMBER(VALUE(LEFT(F1,2))),MID(F1,3,1)="-",ISNUMBER(VALUE(MID(F1,4,6))),MID(F1,10,1)="-",ISNUMBER(VALUE(RIGHT(F1,2)))),AND(LEN(F1)=10,NOT(VALUE(LEFT(F1))=0),ISNUMBER(VALUE(F1))))</formula1>
     </dataValidation>
@@ -759,7 +804,13 @@
       <formula1>=AND(LEN(J2)=2,IF(ISERROR(FIND(",",J2,1)),TRUE,FALSE),IF(ISERROR(FIND("-",J2,1)),TRUE,FALSE),IF(ISERROR(FIND(";",J2,1)),TRUE,FALSE),IF(ISERROR(FIND(CHAR(10),J2,1)),TRUE,FALSE))</formula1>
     </dataValidation>
     <dataValidation sqref="M2:M1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" error="Invalid entry: amount due must not exceed billed amount" type="custom">
-      <formula1>=AND(ISNUMBER(M2), M2 &gt;=0, M2 &lt;= K2)</formula1>
+      <formula1>=AND(ISNUMBER(M2), M2 &gt;=0, M2 &lt;= $K2)</formula1>
+    </dataValidation>
+    <dataValidation sqref="S2:S1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" error="Invalid entry: amount due must not exceed billed amount" type="custom">
+      <formula1>=AND(ISNUMBER(S2), S2 &gt;=0, S2 &lt;= $K2)</formula1>
+    </dataValidation>
+    <dataValidation sqref="P2:P1000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="0" error="Invalid entry: amount due must not exceed billed amount" type="custom">
+      <formula1>=AND(ISNUMBER(P2), P2 &gt;=0, P2 &lt;= $K2)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>